<commit_message>
Elsv QA report accomodated months
</commit_message>
<xml_diff>
--- a/SkillMatrix.Web/wwwroot/Files/Templates/Template_Quality_Elsevier.xlsx
+++ b/SkillMatrix.Web/wwwroot/Files/Templates/Template_Quality_Elsevier.xlsx
@@ -132,7 +132,7 @@
     <t>MJ15</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -180,43 +180,43 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF5050"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF5050"/>
       <name val="Century Gothic"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -550,7 +550,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -660,11 +660,8 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -672,6 +669,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -684,25 +699,19 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -986,7 +995,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -997,12 +1006,12 @@
   <dimension ref="A1:AK1048347"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="56" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="5" width="29.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
@@ -1025,98 +1034,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="41" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="41" t="s">
+      <c r="I1" s="41"/>
+      <c r="J1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="41" t="s">
+      <c r="K1" s="41"/>
+      <c r="L1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="48" t="s">
+      <c r="M1" s="41"/>
+      <c r="N1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="49"/>
-      <c r="P1" s="48" t="s">
+      <c r="O1" s="43"/>
+      <c r="P1" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="48" t="s">
+      <c r="Q1" s="43"/>
+      <c r="R1" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="49"/>
-      <c r="T1" s="50" t="s">
+      <c r="S1" s="43"/>
+      <c r="T1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="51"/>
-      <c r="V1" s="50" t="s">
+      <c r="U1" s="45"/>
+      <c r="V1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="51"/>
-      <c r="X1" s="50" t="s">
+      <c r="W1" s="45"/>
+      <c r="X1" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="52" t="s">
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="52" t="s">
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="52" t="s">
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="53"/>
+      <c r="AE1" s="47"/>
       <c r="AF1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="47" t="s">
+      <c r="AH1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="47" t="s">
+      <c r="AI1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="AJ1" s="47" t="s">
+      <c r="AJ1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="AK1" s="47" t="s">
+      <c r="AK1" s="39" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="30">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="46"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="51"/>
       <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1201,17 +1210,17 @@
       <c r="AG2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="AH2" s="47"/>
-      <c r="AI2" s="47"/>
-      <c r="AJ2" s="47"/>
-      <c r="AK2" s="47"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="39"/>
     </row>
     <row r="3" spans="1:37">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="40">
-        <v>44409</v>
+      <c r="B3" s="54">
+        <v>2021</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>24</v>
@@ -1321,8 +1330,8 @@
       <c r="A4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="40">
-        <v>44409</v>
+      <c r="B4" s="54">
+        <v>2021</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>24</v>
@@ -1434,8 +1443,8 @@
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="40">
-        <v>44409</v>
+      <c r="B5" s="54">
+        <v>2021</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>24</v>
@@ -1547,8 +1556,8 @@
       <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="40">
-        <v>44409</v>
+      <c r="B6" s="54">
+        <v>2021</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>24</v>
@@ -1660,8 +1669,8 @@
       <c r="A7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="40">
-        <v>44409</v>
+      <c r="B7" s="54">
+        <v>2021</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>24</v>
@@ -1769,7 +1778,7 @@
     </row>
     <row r="8" spans="1:37">
       <c r="A8" s="10"/>
-      <c r="B8" s="40"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="11"/>
       <c r="D8" s="12"/>
       <c r="E8" s="37"/>
@@ -1808,7 +1817,7 @@
     </row>
     <row r="9" spans="1:37">
       <c r="A9" s="10"/>
-      <c r="B9" s="40"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
       <c r="E9" s="37"/>
@@ -1847,7 +1856,7 @@
     </row>
     <row r="10" spans="1:37">
       <c r="A10" s="10"/>
-      <c r="B10" s="40"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
       <c r="E10" s="37"/>
@@ -1886,7 +1895,7 @@
     </row>
     <row r="11" spans="1:37">
       <c r="A11" s="10"/>
-      <c r="B11" s="40"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
       <c r="E11" s="37"/>
@@ -1925,7 +1934,7 @@
     </row>
     <row r="12" spans="1:37">
       <c r="A12" s="10"/>
-      <c r="B12" s="40"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="11"/>
       <c r="D12" s="12"/>
       <c r="E12" s="37"/>
@@ -1964,7 +1973,7 @@
     </row>
     <row r="13" spans="1:37">
       <c r="A13" s="10"/>
-      <c r="B13" s="40"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
       <c r="E13" s="37"/>
@@ -2003,7 +2012,7 @@
     </row>
     <row r="14" spans="1:37">
       <c r="A14" s="10"/>
-      <c r="B14" s="40"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="11"/>
       <c r="D14" s="12"/>
       <c r="E14" s="37"/>
@@ -2042,7 +2051,7 @@
     </row>
     <row r="15" spans="1:37">
       <c r="A15" s="10"/>
-      <c r="B15" s="40"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
       <c r="E15" s="37"/>
@@ -2081,7 +2090,7 @@
     </row>
     <row r="16" spans="1:37">
       <c r="A16" s="10"/>
-      <c r="B16" s="40"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="11"/>
       <c r="D16" s="12"/>
       <c r="E16" s="37"/>
@@ -2120,7 +2129,7 @@
     </row>
     <row r="17" spans="1:37">
       <c r="A17" s="10"/>
-      <c r="B17" s="40"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
       <c r="E17" s="37"/>
@@ -2159,7 +2168,7 @@
     </row>
     <row r="18" spans="1:37">
       <c r="A18" s="14"/>
-      <c r="B18" s="40"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
       <c r="E18" s="37"/>
@@ -2198,7 +2207,7 @@
     </row>
     <row r="19" spans="1:37">
       <c r="A19" s="14"/>
-      <c r="B19" s="40"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
       <c r="E19" s="37"/>
@@ -2237,7 +2246,7 @@
     </row>
     <row r="20" spans="1:37">
       <c r="A20" s="14"/>
-      <c r="B20" s="40"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
       <c r="E20" s="37"/>
@@ -2276,7 +2285,7 @@
     </row>
     <row r="21" spans="1:37">
       <c r="A21" s="14"/>
-      <c r="B21" s="40"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="37"/>
@@ -2315,7 +2324,7 @@
     </row>
     <row r="22" spans="1:37">
       <c r="A22" s="14"/>
-      <c r="B22" s="40"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
       <c r="E22" s="37"/>
@@ -2354,7 +2363,7 @@
     </row>
     <row r="23" spans="1:37">
       <c r="A23" s="14"/>
-      <c r="B23" s="40"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
       <c r="E23" s="37"/>
@@ -2393,7 +2402,7 @@
     </row>
     <row r="24" spans="1:37">
       <c r="A24" s="10"/>
-      <c r="B24" s="40"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="37"/>
@@ -2432,7 +2441,7 @@
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="10"/>
-      <c r="B25" s="40"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="37"/>
@@ -2471,7 +2480,7 @@
     </row>
     <row r="26" spans="1:37">
       <c r="A26" s="10"/>
-      <c r="B26" s="40"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="11"/>
       <c r="D26" s="17"/>
       <c r="E26" s="37"/>
@@ -2510,7 +2519,7 @@
     </row>
     <row r="27" spans="1:37">
       <c r="A27" s="10"/>
-      <c r="B27" s="40"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="37"/>
@@ -2549,7 +2558,7 @@
     </row>
     <row r="28" spans="1:37">
       <c r="A28" s="10"/>
-      <c r="B28" s="40"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="37"/>
@@ -2588,7 +2597,7 @@
     </row>
     <row r="29" spans="1:37">
       <c r="A29" s="10"/>
-      <c r="B29" s="40"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="37"/>
@@ -2627,7 +2636,7 @@
     </row>
     <row r="30" spans="1:37">
       <c r="A30" s="10"/>
-      <c r="B30" s="40"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="37"/>
@@ -2666,7 +2675,7 @@
     </row>
     <row r="31" spans="1:37">
       <c r="A31" s="10"/>
-      <c r="B31" s="40"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="37"/>
@@ -2705,7 +2714,7 @@
     </row>
     <row r="32" spans="1:37">
       <c r="A32" s="10"/>
-      <c r="B32" s="40"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="37"/>
@@ -2744,7 +2753,7 @@
     </row>
     <row r="33" spans="1:37">
       <c r="A33" s="10"/>
-      <c r="B33" s="40"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="37"/>
@@ -2783,7 +2792,7 @@
     </row>
     <row r="34" spans="1:37">
       <c r="A34" s="10"/>
-      <c r="B34" s="40"/>
+      <c r="B34" s="54"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="37"/>
@@ -2822,7 +2831,7 @@
     </row>
     <row r="35" spans="1:37">
       <c r="A35" s="10"/>
-      <c r="B35" s="40"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="37"/>
@@ -2861,7 +2870,7 @@
     </row>
     <row r="36" spans="1:37">
       <c r="A36" s="10"/>
-      <c r="B36" s="40"/>
+      <c r="B36" s="54"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="37"/>
@@ -2900,7 +2909,7 @@
     </row>
     <row r="37" spans="1:37">
       <c r="A37" s="10"/>
-      <c r="B37" s="40"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
       <c r="E37" s="37"/>
@@ -2939,7 +2948,7 @@
     </row>
     <row r="38" spans="1:37">
       <c r="A38" s="10"/>
-      <c r="B38" s="40"/>
+      <c r="B38" s="54"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="37"/>
@@ -2978,7 +2987,7 @@
     </row>
     <row r="39" spans="1:37">
       <c r="A39" s="10"/>
-      <c r="B39" s="40"/>
+      <c r="B39" s="54"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="37"/>
@@ -3017,7 +3026,7 @@
     </row>
     <row r="40" spans="1:37">
       <c r="A40" s="10"/>
-      <c r="B40" s="40"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="37"/>
@@ -3056,7 +3065,7 @@
     </row>
     <row r="41" spans="1:37">
       <c r="A41" s="10"/>
-      <c r="B41" s="40"/>
+      <c r="B41" s="54"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="37"/>
@@ -3095,7 +3104,7 @@
     </row>
     <row r="42" spans="1:37">
       <c r="A42" s="10"/>
-      <c r="B42" s="40"/>
+      <c r="B42" s="54"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="37"/>
@@ -3134,7 +3143,7 @@
     </row>
     <row r="43" spans="1:37">
       <c r="A43" s="10"/>
-      <c r="B43" s="40"/>
+      <c r="B43" s="54"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
       <c r="E43" s="37"/>
@@ -3173,7 +3182,7 @@
     </row>
     <row r="44" spans="1:37">
       <c r="A44" s="10"/>
-      <c r="B44" s="40"/>
+      <c r="B44" s="54"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
       <c r="E44" s="37"/>
@@ -3212,7 +3221,7 @@
     </row>
     <row r="45" spans="1:37">
       <c r="A45" s="10"/>
-      <c r="B45" s="40"/>
+      <c r="B45" s="54"/>
       <c r="C45" s="11"/>
       <c r="D45" s="18"/>
       <c r="E45" s="37"/>
@@ -3251,7 +3260,7 @@
     </row>
     <row r="46" spans="1:37">
       <c r="A46" s="10"/>
-      <c r="B46" s="40"/>
+      <c r="B46" s="54"/>
       <c r="C46" s="11"/>
       <c r="D46" s="18"/>
       <c r="E46" s="37"/>
@@ -3290,7 +3299,7 @@
     </row>
     <row r="47" spans="1:37">
       <c r="A47" s="10"/>
-      <c r="B47" s="40"/>
+      <c r="B47" s="54"/>
       <c r="C47" s="11"/>
       <c r="D47" s="18"/>
       <c r="E47" s="37"/>
@@ -3329,7 +3338,7 @@
     </row>
     <row r="48" spans="1:37">
       <c r="A48" s="10"/>
-      <c r="B48" s="40"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="11"/>
       <c r="D48" s="19"/>
       <c r="E48" s="37"/>
@@ -3368,7 +3377,7 @@
     </row>
     <row r="49" spans="1:37">
       <c r="A49" s="10"/>
-      <c r="B49" s="40"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="11"/>
       <c r="D49" s="18"/>
       <c r="E49" s="37"/>
@@ -3407,7 +3416,7 @@
     </row>
     <row r="50" spans="1:37">
       <c r="A50" s="10"/>
-      <c r="B50" s="40"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="11"/>
       <c r="D50" s="19"/>
       <c r="E50" s="37"/>
@@ -3446,7 +3455,7 @@
     </row>
     <row r="51" spans="1:37">
       <c r="A51" s="10"/>
-      <c r="B51" s="40"/>
+      <c r="B51" s="54"/>
       <c r="C51" s="11"/>
       <c r="D51" s="18"/>
       <c r="E51" s="37"/>
@@ -3485,7 +3494,7 @@
     </row>
     <row r="52" spans="1:37">
       <c r="A52" s="10"/>
-      <c r="B52" s="40"/>
+      <c r="B52" s="54"/>
       <c r="C52" s="11"/>
       <c r="D52" s="18"/>
       <c r="E52" s="37"/>
@@ -3524,7 +3533,7 @@
     </row>
     <row r="53" spans="1:37">
       <c r="A53" s="10"/>
-      <c r="B53" s="40"/>
+      <c r="B53" s="54"/>
       <c r="C53" s="11"/>
       <c r="D53" s="19"/>
       <c r="E53" s="37"/>
@@ -3563,7 +3572,7 @@
     </row>
     <row r="54" spans="1:37">
       <c r="A54" s="10"/>
-      <c r="B54" s="40"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="11"/>
       <c r="D54" s="19"/>
       <c r="E54" s="37"/>
@@ -3602,7 +3611,7 @@
     </row>
     <row r="55" spans="1:37">
       <c r="A55" s="10"/>
-      <c r="B55" s="40"/>
+      <c r="B55" s="54"/>
       <c r="C55" s="11"/>
       <c r="D55" s="19"/>
       <c r="E55" s="37"/>
@@ -3641,7 +3650,7 @@
     </row>
     <row r="56" spans="1:37">
       <c r="A56" s="10"/>
-      <c r="B56" s="40"/>
+      <c r="B56" s="54"/>
       <c r="C56" s="11"/>
       <c r="D56" s="18"/>
       <c r="E56" s="37"/>
@@ -3680,7 +3689,7 @@
     </row>
     <row r="57" spans="1:37">
       <c r="A57" s="10"/>
-      <c r="B57" s="40"/>
+      <c r="B57" s="54"/>
       <c r="C57" s="11"/>
       <c r="D57" s="18"/>
       <c r="E57" s="37"/>
@@ -3719,7 +3728,7 @@
     </row>
     <row r="58" spans="1:37">
       <c r="A58" s="10"/>
-      <c r="B58" s="40"/>
+      <c r="B58" s="54"/>
       <c r="C58" s="11"/>
       <c r="D58" s="19"/>
       <c r="E58" s="37"/>
@@ -3758,7 +3767,7 @@
     </row>
     <row r="59" spans="1:37">
       <c r="A59" s="10"/>
-      <c r="B59" s="40"/>
+      <c r="B59" s="54"/>
       <c r="C59" s="11"/>
       <c r="D59" s="19"/>
       <c r="E59" s="37"/>
@@ -3797,7 +3806,7 @@
     </row>
     <row r="60" spans="1:37">
       <c r="A60" s="10"/>
-      <c r="B60" s="40"/>
+      <c r="B60" s="54"/>
       <c r="C60" s="11"/>
       <c r="D60" s="18"/>
       <c r="E60" s="37"/>
@@ -3836,7 +3845,7 @@
     </row>
     <row r="61" spans="1:37">
       <c r="A61" s="10"/>
-      <c r="B61" s="40"/>
+      <c r="B61" s="54"/>
       <c r="C61" s="11"/>
       <c r="D61" s="19"/>
       <c r="E61" s="37"/>
@@ -3875,7 +3884,7 @@
     </row>
     <row r="62" spans="1:37">
       <c r="A62" s="10"/>
-      <c r="B62" s="39"/>
+      <c r="B62" s="55"/>
       <c r="C62" s="11"/>
       <c r="D62" s="34"/>
       <c r="E62" s="38"/>
@@ -3917,6 +3926,14 @@
     <filterColumn colId="1"/>
   </autoFilter>
   <mergeCells count="22">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="AK1:AK2"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
@@ -3931,20 +3948,100 @@
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="2cfe52f1-c433-484a-9b30-91e0bebccbb5">
+      <UserInfo>
+        <DisplayName>Rinos, Regin</DisplayName>
+        <AccountId>46</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Viedor, Eunice Lyn (ELS)</DisplayName>
+        <AccountId>47</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Baider, Roxanne S. (ELS)</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Teresa Frias</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Melissa De Chavez</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Antopina Rosette</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Rhys Palaganas</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Shereen Castillo</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ralph Gil Caguicla</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Corminal, Dain Cain</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Baider Roxanne</DisplayName>
+        <AccountId>20</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Salvador, Gherniel</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Agustin, John Larius</DisplayName>
+        <AccountId>56</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Monwelito Bolandres</DisplayName>
+        <AccountId>27</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100562D7F04798CC943950F971EA3BC3BD9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc9c6569ddc9bb033e0abcb609b35413">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0534b48b-ec10-4412-9d19-d7351618e388" xmlns:ns3="2cfe52f1-c433-484a-9b30-91e0bebccbb5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0eb38ced680094c956cab95dd9100b4" ns2:_="" ns3:_="">
     <xsd:import namespace="0534b48b-ec10-4412-9d19-d7351618e388"/>
@@ -4123,95 +4220,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88006D35-A5FA-437B-A108-419CFA396D01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2cfe52f1-c433-484a-9b30-91e0bebccbb5"/>
+    <ds:schemaRef ds:uri="0534b48b-ec10-4412-9d19-d7351618e388"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="2cfe52f1-c433-484a-9b30-91e0bebccbb5">
-      <UserInfo>
-        <DisplayName>Rinos, Regin</DisplayName>
-        <AccountId>46</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Viedor, Eunice Lyn (ELS)</DisplayName>
-        <AccountId>47</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Baider, Roxanne S. (ELS)</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Teresa Frias</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Melissa De Chavez</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Antopina Rosette</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Rhys Palaganas</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Shereen Castillo</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ralph Gil Caguicla</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Corminal, Dain Cain</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Baider Roxanne</DisplayName>
-        <AccountId>20</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Salvador, Gherniel</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Agustin, John Larius</DisplayName>
-        <AccountId>56</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Monwelito Bolandres</DisplayName>
-        <AccountId>27</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5E8348-75FC-4A58-9B74-8B481C8AB4E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E04D59B7-39C1-44E0-8EE0-1B49B68AE8C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4228,29 +4262,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5E8348-75FC-4A58-9B74-8B481C8AB4E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88006D35-A5FA-437B-A108-419CFA396D01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2cfe52f1-c433-484a-9b30-91e0bebccbb5"/>
-    <ds:schemaRef ds:uri="0534b48b-ec10-4412-9d19-d7351618e388"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>